<commit_message>
Rag version 2 --- en proceso
Version 2 del script que usa chatgpt mini
</commit_message>
<xml_diff>
--- a/notebooks/listado_convocatorias.xlsx
+++ b/notebooks/listado_convocatorias.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -487,39 +487,35 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1050418</v>
+        <v>1051451</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>848857</t>
+          <t>849890</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Resolución del consejero de Educación y Universidades por la cual se convocan ayudas a la red de escuelas infantiles públicas de primer ciclo de las Illes Balears para el año 2025</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Resolució del conseller d’Educació i Universitats per la qual es convoquen ajuts a la xarxa d’escoles infantils públiques de primer cicle de les Illes Balears per a l’any 2025</t>
-        </is>
-      </c>
+          <t>SUBVENCION NOMINATIVA ASOCIACION DE EMPRESARIOS DE TORREDONJIMENO ADET EJERCICIO 2025</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ILLES BALEARS</t>
+          <t>TORREDONJIMENO</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>DIRECCIÓN GENERAL DE INNOVACIÓN Y COMUNIDAD EDUCATIVA</t>
+          <t>AYUNTAMIENTO DE TORREDONJIMENO</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
@@ -527,39 +523,35 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1050417</v>
+        <v>1051450</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>848856</t>
+          <t>849889</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Convocatoria subvenciones SOIB Formación en alternancia en el sector público instrumental, las entidades locales y el tercer sector de acción social 2025-2026</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Convocatòria subvencions SOIB Formació en alternança en el sector públic instrumental, les entitats local i el tercer sector d'acció social 2025-2026</t>
-        </is>
-      </c>
+          <t>ayudas para la ejecución de medidas de promoción del sector vitivinícola en mercados de terceros países y se convocan para el año 2026</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>ILLES BALEARS</t>
+          <t>GALICIA</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>SERVICIO DE OCUPACIÓN DE LAS ISLAS BALEARES (SOIB)</t>
+          <t>CONSELLERÍA DEL MEDIO RURAL</t>
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
@@ -567,35 +559,35 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1050416</v>
+        <v>1051449</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>848855</t>
+          <t>849888</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CONVOCATORIA DEL PROGRAMA PROVINCIAL DE CONSERVACIÓN Y USO DEL PATRIMONIO ARQUEOLÓGICO Y ARQUITECTÓNICO DE LA PROVINCIA DE GRANADA 2025 EN RÉGIMEN DE CONCURRENCIA COMPETITIVA</t>
+          <t>SUBVENCIÓN NOMINATIVA REPOSICIÓN CASETA DE FERIA 2025 "DE JUEVES A VIERNES"</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>DIPUTACIÓN PROV. DE GRANADA</t>
+          <t>CARMONA</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>DIPUTACIÓN PROVINCIAL DE GRANADA</t>
+          <t>AYUNTAMIENTO DE CARMONA</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -603,35 +595,35 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1050415</v>
+        <v>1051448</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>848854</t>
+          <t>849887</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>X2025000101 CONVOCATORIA DE BECAS INDIVIDUALES DE ESCOLARIZACION DURANTE EL AÑO 2025 PARA EL ALUMNADO DE GUARDERÍAS (PRIMER CICLO DE EDUCACIÓN INFANTIL)</t>
+          <t>SUBVENCIÓN NOMINATIVA REPOSICIÓN CASETA DE FERIA 2025 A.C. "EL BOTIJO"</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CASTELLVÍ DE ROSANES</t>
+          <t>CARMONA</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE CASTELLVÍ DE ROSANES</t>
+          <t>AYUNTAMIENTO DE CARMONA</t>
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
@@ -639,35 +631,35 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1050414</v>
+        <v>1051447</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>848853</t>
+          <t>849886</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Convenio de colaboración Federación Galega de Atletismo año 2025</t>
+          <t>SUBVENCIÓN NOMINATIVA REPOSICIÓN CASETA DE FERIA 2025 PEÑA LOS DE LA LUZ</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>SANTIAGO DE COMPOSTELA</t>
+          <t>CARMONA</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE SANTIAGO DE COMPOSTELA</t>
+          <t>AYUNTAMIENTO DE CARMONA</t>
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
@@ -675,35 +667,35 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1050413</v>
+        <v>1051446</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>848852</t>
+          <t>849885</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>X2025000103 CONVOCATORIA AYUDAS DESTINADAS A PALIAR GASTOS DE LA VIVIENDA HABITUAL DE PERSONAS CON EL TÍTULO DE FAMILIA MONOPARENTAL O MONOMARENTAL 2025.</t>
+          <t>SUBVENCIÓN NOMINATIVA REPOSICIÓN CASETA DE FERIA 2025 PEÑA COLUMBICULTORA</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>CASTELLVÍ DE ROSANES</t>
+          <t>CARMONA</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE CASTELLVÍ DE ROSANES</t>
+          <t>AYUNTAMIENTO DE CARMONA</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
@@ -711,167 +703,151 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1050412</v>
+        <v>1051445</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>848851</t>
+          <t>849884</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>I Edición de los Premios Cátedra de Territorios Inteligentes y Sostenibles a los mejores trabajos de final de grado/final de master relacionados con soluciones innovadoras para la mejora de la calidad de vida y sostenibilidad de los municipios de la pro</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>I Edició dels Premis Càtedra de Territoris Intel·ligents i Sostenibles als millors treballs de final de grau o final de màster relacionats amb solucions innovadores per a la millora de la qualitat de vida i sostenibilitat dels municipis de la provín</t>
-        </is>
-      </c>
+          <t>SUBVENCION NOMINATIVA FARMAMUNDI  2025AHE004</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>OTROS</t>
+          <t>ANDALUCÍA</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>UNIVERSITAT DE VALÈNCIA (ESTUDI GENERAL)</t>
+          <t>AGENCIA ANDALUZA DE COOPERACIÓN INTERNACIONAL PARA EL DESARROLLO</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>INV00005380</t>
+          <t>INV00000044</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1050411</v>
+        <v>1051444</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>848850</t>
+          <t>849883</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>VII Edición de los premios de la cátedra de Cooperativas Agroalimentarias de la UV</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>VII Edició del premis de la Càtedra de Cooperatives Agroalimentàries de la UV</t>
-        </is>
-      </c>
+          <t>SUBVENCION NOMINATIVA FAMP 2025</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>OTROS</t>
+          <t>ANDALUCÍA</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>UNIVERSITAT DE VALÈNCIA (ESTUDI GENERAL)</t>
+          <t>AGENCIA ANDALUZA DE COOPERACIÓN INTERNACIONAL PARA EL DESARROLLO</t>
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t>INV00005380</t>
+          <t>INV00000044</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1050410</v>
+        <v>1051443</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>848849</t>
+          <t>849882</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>I Edición del Premio Cátedra AIMPLAS de la Universitat de València al mejor trabajo de Relatos y Cómics Didácticos sobre Sostenibilidad y Economía Circular en el Sector del Plástico</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>I Edició del Premi Càtedra AIMPLAS de la Universitat de València al millor treball de relats i còmics didàctics sobre sostenibilitat i economia circular en el sector del plàstic</t>
-        </is>
-      </c>
+          <t>ORDEN DE 31 DE JULIO DE 2025 POR LA QUE SE APRUEBAN LAS BASES REGULADORAS PARA LA CONCESIÓN DE SUBVENCIONES PARA LA MODERNIZACION DIGITAL DE LOS CENTROS DE TECNIFICACION DEPORTIVA, CENTROS ESPECIALIZADOS DE ALTO RENDIMIENTO Y CENTROS DE ALTO RENDIMIENTO</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>OTROS</t>
+          <t>ANDALUCÍA</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>UNIVERSITAT DE VALÈNCIA (ESTUDI GENERAL)</t>
+          <t>CONSEJERÍA DE CULTURA Y DEPORTE</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>INV00005380</t>
-        </is>
-      </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1050409</v>
+        <v>1051442</v>
       </c>
       <c r="B11" t="b">
         <v>0</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>848848</t>
+          <t>849881</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CONVENIO REGULADOR DE LA CONCESIÓN DE UNA SUBVENCIÓN NOMINATIVA Y DIRECTA AL CDE TWIRLING MAJORETTE CIEMPOZUELOS EN LOS PRESUPUESTOS GENERALES DEL AYUNTAMIENTO DE CIEMPOZUELOS DEL EJERCICIO 2025</t>
+          <t>Resolución de 4 de agosto de 2025, de la D.G. de Trabajo Autónomo y Econ.Social por la que se convocan para los años 2025/26, en rég. de conc.no comp. subvenciones para el fomento del trabajo autónomo, Línea 2 de la Orden de 29.06.2023 - (Mínimi 717/2014.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>CIEMPOZUELOS</t>
+          <t>ANDALUCÍA</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE CIEMPOZUELOS</t>
+          <t>CONSEJERÍA DE EMPLEO, EMPRESA Y TRABAJO AUTÓNOMO</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -879,35 +855,35 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1050408</v>
+        <v>1051441</v>
       </c>
       <c r="B12" t="b">
         <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>848847</t>
+          <t>849880</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>CONVENIO REGULADOR DE LA CONCESIÓN DE UNA SUBVENCIÓN NOMINATIVA Y DIRECTA AL CDE ARCOISCHADIA EN LOS PRESUPUESTOS GENERALES DEL AYUNTAMIENTO DE CIEMPOZUELOS DEL EJERCICIO 2025</t>
+          <t>Resolución de 4 de agosto de 2025, de la D.G. de Trabajo Autónomo y Econ.Social por la que se convocan para los años 2025/26, en rég. de conc.no comp. subvenciones para el fomento del trabajo autónomo, Línea 2 de la Orden de 29.06.2023- (Mínimi 1408/2013)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>CIEMPOZUELOS</t>
+          <t>ANDALUCÍA</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE CIEMPOZUELOS</t>
+          <t>CONSEJERÍA DE EMPLEO, EMPRESA Y TRABAJO AUTÓNOMO</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
@@ -915,79 +891,71 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1050407</v>
+        <v>1051440</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>848846</t>
+          <t>849879</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>XXII Edición del premio de poesia César Simón</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>XXII Edició del premi de poesia César Simón</t>
-        </is>
-      </c>
+          <t>Resolución de 4 de agosto de 2025, de la D.G. de Trabajo Autónomo y Econ.Social por la que se convocan para los años 2025/26, en rég. de conc.no comp. subvenciones para el fomento del trabajo autónomo, Línea 2 de la Orden de 29.06.2023- (Mínimi 1407/2013)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>OTROS</t>
+          <t>ANDALUCÍA</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>UNIVERSITAT DE VALÈNCIA (ESTUDI GENERAL)</t>
+          <t>CONSEJERÍA DE EMPLEO, EMPRESA Y TRABAJO AUTÓNOMO</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>INV00005380</t>
-        </is>
-      </c>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1050406</v>
+        <v>1051439</v>
       </c>
       <c r="B14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>848845</t>
+          <t>849878</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CONVENIO REGULADOR DE LA CONCESIÓN DE UNA SUBVENCIÓN NOMINATIVA Y DIRECTA AL CDE JUDO CIEMPOZUELOS EN LOS PRESUPUESTOS GENERALES DEL AYUNTAMIENTO DE CIEMPOZUELOS DEL EJERCICIO 2025</t>
+          <t>Subvención Excepcional 2024, Conv. Público.  Subv. Directa Excepc. NGP6. Diput. Córdoba. 4 v. La Carlota</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>CIEMPOZUELOS</t>
+          <t>ANDALUCÍA</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE CIEMPOZUELOS</t>
+          <t>CONSEJERÍA DE FOMENTO ARTICULACIÓN DEL TERRITORIO Y VIVIENDA</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -995,159 +963,151 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1050405</v>
+        <v>1051438</v>
       </c>
       <c r="B15" t="b">
         <v>0</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>848844</t>
+          <t>849877</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>C_SUBV_NOM_2025_AYTO_OLIVA DE LA FRONTERA_Pasión Viviente</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
+          <t>RESOLUCIÓN RECTORAL POR LA QUE SE CONVOCAN BECAS DE DESPLAZAMIENTO “OURENSE RURAL-GRADO” PARA ESTUDIANTADO DE GRADO DEL CAMPUS DE OURENSE PARA EL CURSO 2025/2026</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>RESOLUCIÓN REITORAL POLA QUE SE CONVOCAN BOLSAS DE DESPRAZAMENTO “OURENSE RURAL-GRAO” PARA ESTUDANTADO DE GRAO DO CAMPUS DE OURENSE PARA O CURSO 2025/2026</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>DIPUTACIÓN PROV. DE BADAJOZ</t>
+          <t>OTROS</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>DIPUTACIÓN PROVINCIAL DE BADAJOZ</t>
+          <t>UNIVERSIDAD DE VIGO</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>INV00005352</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1050404</v>
+        <v>1051437</v>
       </c>
       <c r="B16" t="b">
         <v>0</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>848843</t>
+          <t>849876</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>IV Edición del premio Cátedra de Joventut de la UV al mejor trabajo fin de grado, trabajo fin de máster y tesis doctoral sobre juventud</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>IV Edició del premi Càtedra de Joventut de la UV al millor treballe fi de grau, treballe fi de màster i tesi doctoral sobre joventut</t>
-        </is>
-      </c>
+          <t>CONVENI CLUB ESPORTIU RIUDEBITLLES</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>OTROS</t>
+          <t>SANT PERE DE RIUDEBITLLES</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>UNIVERSITAT DE VALÈNCIA (ESTUDI GENERAL)</t>
+          <t>AYUNTAMIENTO DE SANT PERE DE RIUDEBITLLES</t>
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>INV00005380</t>
-        </is>
-      </c>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1050403</v>
+        <v>1051436</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>848842</t>
+          <t>849875</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>III Edición de ayudas de la Cátedra de Joventut al mejor proyecto de investigación relacionado con la mejora de la salud mental y la promoción del bienestar en jóvenes</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>III Edició d'ajudes de la Càtedra de Joventut al millor projecte d'investigació relacionat amb la millora de la salut mental i la promoció del benestar en joves</t>
-        </is>
-      </c>
+          <t>CONVENI CARITAS</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>OTROS</t>
+          <t>SANT PERE DE RIUDEBITLLES</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>UNIVERSITAT DE VALÈNCIA (ESTUDI GENERAL)</t>
+          <t>AYUNTAMIENTO DE SANT PERE DE RIUDEBITLLES</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>INV00005380</t>
-        </is>
-      </c>
+      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1050402</v>
+        <v>1051435</v>
       </c>
       <c r="B18" t="b">
         <v>0</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>848841</t>
+          <t>849874</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Subvención nominativa Associació Joventuts Musicals de la Bisbal d'Empordà - actividad anual 2025</t>
+          <t>Resolución Dirección SCE concesión/denegación becas/ayudas alum. desemp. cursos ocupados prog.2024 Fichero 11</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>BISBAL D'EMPORDÀ, LA</t>
+          <t>CANARIAS</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE BISBAL D'EMPORDÀ, LA</t>
+          <t>SERVICIO CANARIO DE EMPLEO</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
@@ -1155,35 +1115,35 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1050401</v>
+        <v>1051434</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>848840</t>
+          <t>849873</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Convenio entre la Diputación Provincial de Teruel, la Fundación Bancaria Ibercaja y el Obispado de Teruel y Albarracín para restauración del patrimonio artístico religioso de la Diócesis de Teruel y Albarracín</t>
+          <t>Ayuda Emergencia Social 2025</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>DIPUTACIÓN PROV. DE TERUEL</t>
+          <t>CANARIAS</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>DIPUTACIÓN PROVINCIAL DE TERUEL</t>
+          <t>CONSEJERÍA DE BIENESTAR SOCIAL, IGUALDAD, JUVENTUD, INFANCIA Y FAMILIAS</t>
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
@@ -1191,25 +1151,25 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1050400</v>
+        <v>1051433</v>
       </c>
       <c r="B20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>848839</t>
+          <t>849872</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Subvención promoción y difusión ACREDITA, CCE 2025</t>
+          <t>SDF2023TF00126 AYUDAS DE EMERGENCIA SOCIAL 2025</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1219,7 +1179,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>CONSEJERÍA DE EDUCACIÓN, FORMACIÓN PROFESIONAL, ACTIVIDAD FÍSICA Y DEPORTES</t>
+          <t>CONSEJERÍA DE BIENESTAR SOCIAL, IGUALDAD, JUVENTUD, INFANCIA Y FAMILIAS</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
@@ -1227,25 +1187,25 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1050399</v>
+        <v>1051432</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>848838</t>
+          <t>849871</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Concesión de becas y ayudas destinadas a la realización de acciones formativas dirigidas prioritariamente a personas trabajadoras desempleadas incluidas en la programación 2025</t>
+          <t>Ayuda Emergencia Social 2025</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1255,7 +1215,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>SERVICIO CANARIO DE EMPLEO</t>
+          <t>CONSEJERÍA DE BIENESTAR SOCIAL, IGUALDAD, JUVENTUD, INFANCIA Y FAMILIAS</t>
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
@@ -1263,25 +1223,25 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1050398</v>
+        <v>1051431</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>848837</t>
+          <t>849870</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Hermandad Ntra. Sra. de las Nieves_Festividad virgen de las Nieves</t>
+          <t>SDF2025TF00052 Ayudas de emergencia social 2025</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1291,7 +1251,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>PRESIDENCIA DEL GOBIERNO</t>
+          <t>CONSEJERÍA DE BIENESTAR SOCIAL, IGUALDAD, JUVENTUD, INFANCIA Y FAMILIAS</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
@@ -1299,25 +1259,25 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1050397</v>
+        <v>1051430</v>
       </c>
       <c r="B23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>848836</t>
+          <t>849869</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>orden de 6 de  mayo 2024 se convocan las subvenciones destinadas reconstruccion potencial por incendios en la Palma y Tenerife</t>
+          <t>Subvención promoción y difusión ACREDITA, CCE 2025 def</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1327,7 +1287,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>CONSEJERÍA DE AGRICULTURA, GANADERÍA, PESCA Y SOBERANÍA ALIMENTARIA</t>
+          <t>CONSEJERÍA DE EDUCACIÓN, FORMACIÓN PROFESIONAL, ACTIVIDAD FÍSICA Y DEPORTES</t>
         </is>
       </c>
       <c r="I23" t="inlineStr"/>
@@ -1335,35 +1295,35 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1050396</v>
+        <v>1051429</v>
       </c>
       <c r="B24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>848835</t>
+          <t>849868</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Subvención nominativa a la entidad FALLA  EL POBLE 2025</t>
+          <t>Subvención promoción y difusión ACREDITA, CCOO 2025</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>MASSANASSA</t>
+          <t>CANARIAS</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE MASSANASSA</t>
+          <t>CONSEJERÍA DE EDUCACIÓN, FORMACIÓN PROFESIONAL, ACTIVIDAD FÍSICA Y DEPORTES</t>
         </is>
       </c>
       <c r="I24" t="inlineStr"/>
@@ -1371,35 +1331,35 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1050394</v>
+        <v>1051428</v>
       </c>
       <c r="B25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>848833</t>
+          <t>849867</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Subvención nominativa a la entidad COFRADIA SANTISIMO CRISTO DE LA VIDA 2025</t>
+          <t>Subvención promoción y difusión ACREDITA, UGT 2025</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>MASSANASSA</t>
+          <t>CANARIAS</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE MASSANASSA</t>
+          <t>CONSEJERÍA DE EDUCACIÓN, FORMACIÓN PROFESIONAL, ACTIVIDAD FÍSICA Y DEPORTES</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
@@ -1407,35 +1367,35 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1050393</v>
+        <v>1051427</v>
       </c>
       <c r="B26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>848832</t>
+          <t>849866</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Subvención nominativa a la entidad ASOCIACIÓN CULTURAL FALLA DIVENDRES para 2025</t>
+          <t>Subvención promoción y difusión ACREDITA, CPESCT 2025</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>MASSANASSA</t>
+          <t>CANARIAS</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE MASSANASSA</t>
+          <t>CONSEJERÍA DE EDUCACIÓN, FORMACIÓN PROFESIONAL, ACTIVIDAD FÍSICA Y DEPORTES</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
@@ -1443,35 +1403,35 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1050392</v>
+        <v>1051426</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>848831</t>
+          <t>849865</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>CONVOCATORIA XIV CERTAMEN DE PINTURA RÁPIDA PARLA ALAYRE 2025</t>
+          <t>NOMINADAS 2025</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>PARLA</t>
+          <t>CANARIAS</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE PARLA</t>
+          <t>CONSEJERÍA DE BIENESTAR SOCIAL, IGUALDAD, JUVENTUD, INFANCIA Y FAMILIAS</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -1479,35 +1439,35 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1050391</v>
+        <v>1051425</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>848830</t>
+          <t>849864</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>SUBVENCION NOMINATIVA CLUB NATACIO VALLIRANA AÑO 2025</t>
+          <t>Subvención Directa Compensación Medidas Fitotanitarias Virus Rugoso del Tomate</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>VALLIRANA</t>
+          <t>CANARIAS</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE VALLIRANA</t>
+          <t>CONSEJERÍA DE AGRICULTURA, GANADERÍA, PESCA Y SOBERANÍA ALIMENTARIA</t>
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
@@ -1515,35 +1475,35 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1050390</v>
+        <v>1051424</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>848829</t>
+          <t>849863</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Convocatoria Subvenciones participación XXVIII Muestra Local de Teatro de 2025 a entidades ciudadanas del Ayuntamiento de Parla</t>
+          <t>gastos generales</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>PARLA</t>
+          <t>CANARIAS</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE PARLA</t>
+          <t>PRESIDENCIA DEL GOBIERNO</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
@@ -1551,35 +1511,35 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1050389</v>
+        <v>1051423</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>848828</t>
+          <t>849862</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Concesión de subvención nominativa 2025 a la entidad Colla Despertades</t>
+          <t>ULPGC Programa predoctoral 2025</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>MASSANASSA</t>
+          <t>CANARIAS</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE MASSANASSA</t>
+          <t>CONSEJERÍA DE UNIVERSIDADES, CIENCIA E INNOVACIÓN Y CULTURA</t>
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
@@ -1587,39 +1547,35 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1050388</v>
+        <v>1051422</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>848827</t>
+          <t>849861</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Subvención nominativa a favor del Club de Futbol Ponent.</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Subvenció nominativa a favor del Club de Futbol Ponent.</t>
-        </is>
-      </c>
+          <t>LÍNEA 2 INCENTIVOS CANARIOS 2025</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>GRANOLLERS</t>
+          <t>CANARIAS</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE GRANOLLERS</t>
+          <t>CONSEJERÍA DE ECONOMÍA, INDUSTRIA, COMERCIO Y AUTÓNOMOS</t>
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
@@ -1627,39 +1583,35 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1050386</v>
+        <v>1051421</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>848825</t>
+          <t>849860</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Subvención nominativa a favor de l'Associació Granollers Esportiva</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Subvenció nominativa a favor de l'Associació Granollers Esportiva</t>
-        </is>
-      </c>
+          <t>Convocatoria Parados de larga Duración 2025</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>GRANOLLERS</t>
+          <t>CANARIAS</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE GRANOLLERS</t>
+          <t>SERVICIO CANARIO DE EMPLEO</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
@@ -1667,39 +1619,35 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1050385</v>
+        <v>1051420</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>848824</t>
+          <t>849859</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Subvención nominativa a favor de la entidad Unió General de Treballadores i Treballadors de Catalunya.</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Subvenció nominativa a favor de l'entitat Unió General de Treballadores i Treballadors de Catalunya.</t>
-        </is>
-      </c>
+          <t>PROGRAMAS INTERES GENERAL ASIGNACION TRIBUTAIRA IRPF</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>GRANOLLERS</t>
+          <t>CANARIAS</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE GRANOLLERS</t>
+          <t>CONSEJERÍA DE BIENESTAR SOCIAL, IGUALDAD, JUVENTUD, INFANCIA Y FAMILIAS</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
@@ -1707,79 +1655,71 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1050384</v>
+        <v>1051419</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>848823</t>
+          <t>849858</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Bonificaciones al transporte marítimo regular de pasajeros miembros de FAMILIAS NUMEROSAS 2024</t>
+          <t>Resolución por la que se aprueba la convocatoria de concesión de ayudas para el impulso empresarial de autónomos, microempresas, pequeñas y medianas empresas con establecimiento permanente en el Principado de Asturias en el año 2025</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>ESTADO</t>
+          <t>PRINCIPADO DE ASTURIAS</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>MINISTERIO DE TRANSPORTES Y MOVILIDAD SOSTENIBLE</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>DIRECCIÓN GENERAL DE LA MARINA MERCANTE</t>
-        </is>
-      </c>
+          <t>CONSEJERÍA DE CIENCIA, EMPRESAS, FORMACIÓN Y EMPLEO</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1050383</v>
+        <v>1051418</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>848822</t>
+          <t>849857</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>SUBVENCIÓN NOMINATIVA DIOCESIS DE LUGO PARA LA  REHABILITACIÓN DE LA CAPILLA DEL CARMEN</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>SUBVENCIÓN NOMINATIVA DIOCESE DE LUGO PARA A  REHABILITACIÓN DA CAPELA DO CARME</t>
-        </is>
-      </c>
+          <t>BOGHÉ VERDE: DESARROLLO SOSTENIBLE Y GESTIÓN ECOLÓGICA DE LOS ESPACIOS URBANOS EN EL MARCO DEL APOYO A LA REFORMA NORMATIVA Y COMPETENCIAS LOCALES EN MAURITANIA</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>LUGO</t>
+          <t>DIPUTACIÓN PROV. DE JAÉN</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>CONCELLO DE LUGO</t>
+          <t>DIPUTACIÓN PROVINCIAL DE JAÉN</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
@@ -1787,35 +1727,35 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1050382</v>
+        <v>1051417</v>
       </c>
       <c r="B36" t="b">
         <v>0</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>848821</t>
+          <t>849856</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Concesión de subvención directa a la Parroquia de San Bartolomé 2025</t>
+          <t>FORTALECIMIENTO DE LA ESTRATEGIA DE APOYO MUNICIPAL EN REPÚBLICA DOMINICANA: GESTIÓN INTEGRAL DE RESIDUOS SÓLIDOS Y DESARROLLO ECONÓMICO LOCAL</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>ALDEANUEVA DE EBRO</t>
+          <t>DIPUTACIÓN PROV. DE JAÉN</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE ALDEANUEVA DE EBRO</t>
+          <t>DIPUTACIÓN PROVINCIAL DE JAÉN</t>
         </is>
       </c>
       <c r="I36" t="inlineStr"/>
@@ -1823,79 +1763,71 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1050381</v>
+        <v>1051416</v>
       </c>
       <c r="B37" t="b">
         <v>0</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>848820</t>
+          <t>849855</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Bonificaciones al transporte marítimo regular de pasajeros RESIDENTES extrapeninsulares 2024</t>
+          <t>LECTURAS VERDES: UN VIAJE HACIA LA SOSTENIBILIDAD EN LA PROVINCIA DE JAÉN.' PROGRAMA DE SENSIBILIZACIÓN CIUDADANA PARA LA LUCHA CONTRA EL CAMBIO CLIMÁTICO A TRAVÉS DE LA LECTURA</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>ESTADO</t>
+          <t>DIPUTACIÓN PROV. DE JAÉN</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>MINISTERIO DE TRANSPORTES Y MOVILIDAD SOSTENIBLE</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>DIRECCIÓN GENERAL DE LA MARINA MERCANTE</t>
-        </is>
-      </c>
+          <t>DIPUTACIÓN PROVINCIAL DE JAÉN</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1050379</v>
+        <v>1051414</v>
       </c>
       <c r="B38" t="b">
         <v>0</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>848818</t>
+          <t>849853</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Resolución por la que se abre la convocatoria 2025 para la concesión de subvenciones, en régimen de concurrencia competitiva, para incentivar la presencia de artistas catalanes en el ámbito de la música en México.</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>Resolució per la qual s’obre la convocatòria 2025 per a la concessió de subvencions, en règim de concurrència competitiva, per incentivar la presència d'artistes catalans en l'àmbit de la música a Mèxic</t>
-        </is>
-      </c>
+          <t>JUNTA DE GOBIERNO DE 30/07/2025 QUE APRUEBA LA CONVOCATORIA SUBVENCIONES PARA EL I CONCURSO DE FOTOGRAFÍA “CALENDARIO DE FIESTAS TRADICIONALES DE GUADALAJARA</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>CATALUÑA</t>
+          <t>DIPUTACIÓN PROV. DE GUADALAJARA</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>INSTITUT RAMON LLULL</t>
+          <t>DIPUTACIÓN PROVINCIAL DE GUADALAJARA</t>
         </is>
       </c>
       <c r="I38" t="inlineStr"/>
@@ -1903,35 +1835,39 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1050378</v>
+        <v>1051413</v>
       </c>
       <c r="B39" t="b">
         <v>0</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>848817</t>
+          <t>849852</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>CONVOCATORIA DE SUBVENCIÓN NOMINATIVA A FAVOR DE LA UNIÓN PROVINCIAL CORDOBESA DE VENTA AMBULANTE (UPCOVA), PARA LA REALIZACIÓN DEL PROYECTO “FORTALECIMIENTO ASOCIATIVO Y PROMOCIÓN DEL COMERCIO AMBULANTE LOCAL”.</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr"/>
+          <t>BASES ESPECÍFICAS DEL VIII CERTAMEN DE POESÍA TORRE DE CALDALOBA (AYUNTAMIENTO DE COSPEITO) Y CONVOCATORIA</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>BASES ESPECÍFICAS DO VIII CERTAME DE POESÍA TORRE DE CALDALOBA (CONCELLO DE COSPEITO) E CONVOCATORIA</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>CÓRDOBA</t>
+          <t>COSPEITO</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE CÓRDOBA</t>
+          <t>AYUNTAMIENTO DE COSPEITO</t>
         </is>
       </c>
       <c r="I39" t="inlineStr"/>
@@ -1939,71 +1875,75 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1050377</v>
+        <v>1051412</v>
       </c>
       <c r="B40" t="b">
         <v>0</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>848816</t>
+          <t>849851</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>SUBVENCIÓN NOMINATIVA ASOCIACION DE VECINOS GRUPO FATIMA 2025</t>
+          <t>CONVENIO DE COLABORACIÓN ENTRE EL INSTITUTO ARAGONÉS DE LA MUJER Y EL CONSEJO DE COLEGIOS DE ABOGADOS DE ARAGÓN PARA LA PRESTACIÓN DEL SERVICIO DE ASESORAMIENTO JURÍDICO INDIVIDUALIZADO A MUJERES</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>ALMASSORA</t>
+          <t>ARAGÓN</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE ALMAZORA/ALMASSORA</t>
+          <t>INSTITUTO ARAGONÉS DE LA MUJER (IAM)</t>
         </is>
       </c>
       <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr"/>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>INV00003656</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1050376</v>
+        <v>1051411</v>
       </c>
       <c r="B41" t="b">
         <v>0</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>848815</t>
+          <t>849850</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>CONVENIO 2024 ASOCIACIÓN JUDO Y D.A ATENEU DE VILASSAR DE MAR</t>
+          <t>2ª PRÓRROGA CONVENIO SAN JUAN DE DIOS</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>VILASSAR DE MAR</t>
+          <t>VALENCIA</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE VILASSAR DE MAR</t>
+          <t>AYUNTAMIENTO DE VALENCIA</t>
         </is>
       </c>
       <c r="I41" t="inlineStr"/>
@@ -2011,39 +1951,35 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1050375</v>
+        <v>1051410</v>
       </c>
       <c r="B42" t="b">
         <v>0</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>848814</t>
+          <t>849849</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Otorgar la subvención nominativa a la Associación Cultural de Granollers para su proyecto Big Band Granollers, Rueda de Espectaculos y Centros de Estudios 2025</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Atorgar la subvenció nominativa a l'Associació Cultural de Granollers per al seu projecte Big Band Granollers, Roda d'Espectacles i Centres d'Estudis 2025</t>
-        </is>
-      </c>
+          <t>Convocatoria Subvenciones Nominativas Ejercicio 2024 Unión Musical de Moncada</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>GRANOLLERS</t>
+          <t>MONCADA</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE GRANOLLERS</t>
+          <t>AYUNTAMIENTO DE MONCADA</t>
         </is>
       </c>
       <c r="I42" t="inlineStr"/>
@@ -2051,35 +1987,35 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1050374</v>
+        <v>1051409</v>
       </c>
       <c r="B43" t="b">
         <v>0</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>848813</t>
+          <t>849848</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>BASES REGULADORAS Y CONVOCATORIA DEL PROGRAMA “BO COMERÇ D’ALMUSSAFES 2025” PARA LA RECUPERACIÓN DEL SECTOR COMERCIAL Y SERVICIOS DE ALMUSSAFES</t>
+          <t>Subvención nominativa al Club de Ajedrez Dama de Guardamar. Anualidad 2025.</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>ALMUSSAFES</t>
+          <t>GUARDAMAR DEL SEGURA</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE ALMUSSAFES</t>
+          <t>AYUNTAMIENTO DE GUARDAMAR DEL SEGURA</t>
         </is>
       </c>
       <c r="I43" t="inlineStr"/>
@@ -2087,39 +2023,35 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1050373</v>
+        <v>1051408</v>
       </c>
       <c r="B44" t="b">
         <v>0</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>848812</t>
+          <t>849847</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Aprobar el otorgamiento de una subvención nominativa a favor de la entidad Minyons Escoltes y Guies Sant Jordi de Catalunya, por actividades que desarrolla el Agrupament Escolta y Guía Sant Esteve de Granollers para el proyecto Campamentos de verano para</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>Aprovar l'atorgament d'una subvenció nominativa a favor de l'entitat Minyons Escoltes i Guies Sant Jordi de Catalunya, per activitats que desenvolupa l'Agrupament Escolta i Guia Sant Esteve de Granollers pel projecte Campaments d¿estiu per l¿any 2025</t>
-        </is>
-      </c>
+          <t>Concesión Subvenciones Nominativas Ejercicio 2024 Centro Artístico Musical</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>GRANOLLERS</t>
+          <t>MONCADA</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE GRANOLLERS</t>
+          <t>AYUNTAMIENTO DE MONCADA</t>
         </is>
       </c>
       <c r="I44" t="inlineStr"/>
@@ -2127,36 +2059,35 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1050372</v>
+        <v>1051407</v>
       </c>
       <c r="B45" t="b">
         <v>0</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>848811</t>
+          <t>849846</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Subvención Directa, mediante Convenio, con Club Deportivo Aldeano para la financiación de los gastos derivados del desarrollo de la
-actividad deportiva durante el año 2025</t>
+          <t>SUBVENCIÓN DIRECTA OTORGADA A FAVOR DE AYUNTAMIENTO DE VILLERIAS DE CAMPOS PARA REPARACIÓN CUBIERTA Y MEJORA DEL CENTRO CULTURAL</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>ALDEANUEVA DE EBRO</t>
+          <t>DIPUTACIÓN PROV. DE PALENCIA</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE ALDEANUEVA DE EBRO</t>
+          <t>DIPUTACIÓN PROVINCIAL DE PALENCIA</t>
         </is>
       </c>
       <c r="I45" t="inlineStr"/>
@@ -2164,35 +2095,35 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1050371</v>
+        <v>1051406</v>
       </c>
       <c r="B46" t="b">
         <v>0</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>848810</t>
+          <t>849845</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Subv. CEBC Olimpiada Escolar 2025</t>
+          <t>Convenio entre la Vicepresidencia 2ª y el Ayuntamiento de Almedina (CR) para subvención en materia de memoria democrática 2025.</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>REUS</t>
+          <t>CASTILLA-LA MANCHA</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE REUS</t>
+          <t>VICECONSEJERÍA DE RELACIONES INSTITUCIONALES</t>
         </is>
       </c>
       <c r="I46" t="inlineStr"/>
@@ -2200,35 +2131,35 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1050370</v>
+        <v>1051405</v>
       </c>
       <c r="B47" t="b">
         <v>0</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>848809</t>
+          <t>849844</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Convenio de colaboración entre el Ayuntamiento de Collado Mediano y el CEIP “VIRGEN DE LA PAZ” de Collado Mediano. Año 2025. Subvención nominativa</t>
+          <t>CONVOCATORIA SUBVENCIÓ A.D.N. AGRUPACIÓ DEFENSA DE LA NATURA DELS MONJOS. ANY 2025</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>COLLADO MEDIANO</t>
+          <t>SANTA MARGARIDA I ELS MONJOS</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE COLLADO MEDIANO</t>
+          <t>AYUNTAMIENTO DE SANTA MARGARIDA I ELS MONJOS</t>
         </is>
       </c>
       <c r="I47" t="inlineStr"/>
@@ -2236,39 +2167,35 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1050369</v>
+        <v>1051404</v>
       </c>
       <c r="B48" t="b">
         <v>0</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>848808</t>
+          <t>849843</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Aprovar l'atorgament d'una subvenció nominativa a favor de l'escola Joan Solans destinada a desenvolupar el projecte: Activitats culturals, de descoberta i de joc per a tots els alumnes de l'escola, 2025</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>Aprovar l'atorgament d'una subvenció nominativa a favor de l'escola Joan Solans destinada a desenvolupar el projecte: Activitats culturals, de descoberta i de joc per a tots els alumnes de l'escola, 2025</t>
-        </is>
-      </c>
+          <t>CONVOCATORIA SUBVENCIÓ AGRUPACIO DE DEFENSA FORESTAL PUIG DE L¿ÀGUILA ANY 2025</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>GRANOLLERS</t>
+          <t>SANTA MARGARIDA I ELS MONJOS</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE GRANOLLERS</t>
+          <t>AYUNTAMIENTO DE SANTA MARGARIDA I ELS MONJOS</t>
         </is>
       </c>
       <c r="I48" t="inlineStr"/>
@@ -2276,35 +2203,35 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1050368</v>
+        <v>1051403</v>
       </c>
       <c r="B49" t="b">
         <v>0</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>848807</t>
+          <t>849842</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>CONVENIO DE COLABORACIÓN ENTRE EL ILUSTRE AYUNTAMIENTO DE  TOTANA Y LA CORAL SANTIAGO DE TOTANA PARA EL AÑO 2025</t>
+          <t>SUBVENCIÓN PREMIOS CONCURSO LOCAL PINTURA FIESTA MAYOR PALLEJÀ 2025</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>TOTANA</t>
+          <t>PALLEJÀ</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE TOTANA</t>
+          <t>AYUNTAMIENTO DE PALLEJÀ</t>
         </is>
       </c>
       <c r="I49" t="inlineStr"/>
@@ -2312,35 +2239,35 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1050367</v>
+        <v>1051402</v>
       </c>
       <c r="B50" t="b">
         <v>0</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>848806</t>
+          <t>849841</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>SUBVENCION NOMINATIVA LILCAM</t>
+          <t>Convocatoria Subvenciones Nominativas Ejercicio 2024 Associació Cultural Anidea Teatre</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>CASTILLA-LA MANCHA</t>
+          <t>MONCADA</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>DIRECCION GENERAL ORDENACION AGROPECUARIA</t>
+          <t>AYUNTAMIENTO DE MONCADA</t>
         </is>
       </c>
       <c r="I50" t="inlineStr"/>
@@ -2348,39 +2275,35 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1050366</v>
+        <v>1051401</v>
       </c>
       <c r="B51" t="b">
         <v>0</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>848805</t>
+          <t>849840</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>RESOLUCIÓN de 17 de julio de 2025, por la que se conceden ayudas a la Fundación Valenciana Premios Rei Jaume I de la Comunitat Valenciana (línea de subvención S0671) para el ejercicio 2025</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>RESOLUCIÓ de 17 de juliol del 2025, per la qual es concedixen ajudes a la Fundació Valenciana Premis Rei Jaume I de la Comunitat Valenciana (línia de subvenció S0671) per a l’exercici 2025.</t>
-        </is>
-      </c>
+          <t>SUBVENCIÓN DIRECTA OTORGADA A FAVOR DE AYUNTAMIENTO DE BASCONES DE OJEDA RENOVACION ALUMBRADO PUBLICO POR TECNOLOGIA LED</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>COMUNITAT VALENCIANA</t>
+          <t>DIPUTACIÓN PROV. DE PALENCIA</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>SECRETARIA AUTONÓMICA DEL GABINETE DEL PRESIDENT Y COMUNICACIÓN</t>
+          <t>DIPUTACIÓN PROVINCIAL DE PALENCIA</t>
         </is>
       </c>
       <c r="I51" t="inlineStr"/>
@@ -2388,35 +2311,35 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1050365</v>
+        <v>1051400</v>
       </c>
       <c r="B52" t="b">
         <v>0</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>848804</t>
+          <t>849839</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>SUBVENCIÓN NOMINATIVA AL CB CRIPTANA JUNIOR FEMENINO PARA EL DESPLAZAMIENTO A HUELVA EN EL CAMPEONATO DE ESPAÑA JUNIOR DE BALONCESTO.</t>
+          <t>CONVOCATORIA SUBVENCIÓ GRUP ESTUDIS RAPITENCS. ANY 2025</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>DIPUTACIÓN PROV. DE CIUDAD REAL</t>
+          <t>SANTA MARGARIDA I ELS MONJOS</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>DIPUTACIÓN PROVINCIAL DE CIUDAD REAL</t>
+          <t>AYUNTAMIENTO DE SANTA MARGARIDA I ELS MONJOS</t>
         </is>
       </c>
       <c r="I52" t="inlineStr"/>
@@ -2424,35 +2347,35 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1050364</v>
+        <v>1051399</v>
       </c>
       <c r="B53" t="b">
         <v>0</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>848803</t>
+          <t>849838</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>CONVENIO DE COLABORACIÓN ENTRE EL AYUNTAMIENTO DE TOTANA Y LA PARROQUIA DE SANTIAGO EL MAYOR DE TOTANA PARA LA REALIZACIÓN DE ACCIONES DE INTERÉS SOCIAL DESARROLLADAS POR CÁRITAS PARROQUIEL EN EL MUNICIPIO DE TOTANA.- AÑO 2025</t>
+          <t>SUBV. DIRECTA EXCEPCIONAL A LA FUNDACIÓN MUSICAL DE MÁLAGA, PROYECTO "XVI CICLO DE CONCIERTOS DIDÁCTICOS"</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>TOTANA</t>
+          <t>MÁLAGA</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE TOTANA</t>
+          <t>AYUNTAMIENTO DE MÁLAGA</t>
         </is>
       </c>
       <c r="I53" t="inlineStr"/>
@@ -2460,39 +2383,35 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1050363</v>
+        <v>1051398</v>
       </c>
       <c r="B54" t="b">
         <v>0</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>848802</t>
+          <t>849837</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Aprobar una subvención nominativa a favor de la entidad Sociedad Coral Amics de la Unió, destinada al desarrollo y ejecución del casal Estancias Musicales incluido en el programa Hazte el Verano para el año 2025.</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>Aprovar una subvenció nominativa a favor del l'entitat Societat Coral Amics de la Unió, destinada al desenvolupament i execució del casal Estades Musicals inclòs al programa Fes-te l'Estiu per l'any 2025.</t>
-        </is>
-      </c>
+          <t>CONCURSO DE ESCAPARATES FIESTAS PATRONALES 2025</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>GRANOLLERS</t>
+          <t>SEGORBE</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE GRANOLLERS</t>
+          <t>AYUNTAMIENTO DE SEGORBE</t>
         </is>
       </c>
       <c r="I54" t="inlineStr"/>
@@ -2500,39 +2419,39 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1050362</v>
+        <v>1051396</v>
       </c>
       <c r="B55" t="b">
         <v>0</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>848801</t>
+          <t>849835</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Financiación del proyecto "Comunidad Decidim: Fortalecimiento y coordinación de la gobernanza participativa", de la Associació de Software Lliure Decidim, previsto para el año 2025.</t>
+          <t>Convocatoria de subvención a URV PROY. POBLADO VISIGÓTICO ROSES, ejercicio 2025.</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Finanament del projecte Comunitat Decidim: Enfortiment i coordinació de la governana participativa, de l'Associació de Software Lliure Decidim, previst per a l'any 2025.</t>
+          <t>Convocatòria de subvenció a UDG PROJ. POBLAT VISIGÒTIC ROSES, exercici 2025.</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>CATALUÑA</t>
+          <t>ROSES</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>DEPARTAMENT DE LA PRESIDÈNCIA</t>
+          <t>AYUNTAMIENTO DE ROSES</t>
         </is>
       </c>
       <c r="I55" t="inlineStr"/>
@@ -2540,36 +2459,39 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1050361</v>
+        <v>1051395</v>
       </c>
       <c r="B56" t="b">
         <v>0</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>848800</t>
+          <t>849834</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t xml:space="preserve">EXPEDIENTE 2278282F: CONCESIÓN SUBVENCIÓN A SOCIEDAD CIVIL PARTICULAR EL PINAR SEGÚN BASE 30.10 DEL PRESUPUESTO MUNICIPAL EJERCICIO 2025.
-</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr"/>
+          <t>Ayudas dirigidas al desarrollo de proyectos de descarbonización 2025</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Deskarbonizazio-proiektuak garatzeko laguntzak 2025</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>PICASSENT</t>
+          <t>VITORIA-GASTEIZ</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE PICASSENT</t>
+          <t>AYUNTAMIENTO DE VITORIA-GASTEIZ</t>
         </is>
       </c>
       <c r="I56" t="inlineStr"/>
@@ -2577,35 +2499,35 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1050360</v>
+        <v>1051394</v>
       </c>
       <c r="B57" t="b">
         <v>0</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>848799</t>
+          <t>849833</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Convenio de colaboración Club Ciclista Compostelano año 2025</t>
+          <t>Convocatoria Subvenciones Nominativas Ejercicio 2024 Asociación Cultural Juguem al Truc</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>SANTIAGO DE COMPOSTELA</t>
+          <t>MONCADA</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE SANTIAGO DE COMPOSTELA</t>
+          <t>AYUNTAMIENTO DE MONCADA</t>
         </is>
       </c>
       <c r="I57" t="inlineStr"/>
@@ -2613,35 +2535,39 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1050359</v>
+        <v>1051393</v>
       </c>
       <c r="B58" t="b">
         <v>0</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>848798</t>
+          <t>849832</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>SUBVENCIÓN NOMINATIVA FUNDACIÓ ANA RIBOT 2025</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr"/>
+          <t>Convocatoria de subvenciones para el uso del euskera en la rotulación, imagen corporativa y páginas web de establecimientos comerciales, así como páginas web de clubes deportivos.</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Zizur Nagusiko merkataritza establezimenduetako errotulazioan, irudi korporatiboan eta web orrietan, baita Zizur Nagusiko kirol kluben webguneetan euskararen erabilera laguntzeko dirulaguntzen deialdia</t>
+        </is>
+      </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>PALLEJÀ</t>
+          <t>ZIZUR MAYOR/ZIZUR NAGUSIA</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE PALLEJÀ</t>
+          <t>AYUNTAMIENTO DE ZIZUR MAYOR/ZIZUR NAGUSIA</t>
         </is>
       </c>
       <c r="I58" t="inlineStr"/>
@@ -2649,35 +2575,35 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1050358</v>
+        <v>1051392</v>
       </c>
       <c r="B59" t="b">
         <v>0</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>848797</t>
+          <t>849831</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Subvención a la Asociación Hermandad de la Verónica</t>
+          <t>“PREMIOS PROVINCIALES DE LA SOLIDARIDAD 2025”</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>HELLÍN</t>
+          <t>DIPUTACIÓN PROV. DE ALICANTE</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE HELLÍN</t>
+          <t>DIPUTACIÓN PROVINCIAL DE ALACANT/ALICANTE</t>
         </is>
       </c>
       <c r="I59" t="inlineStr"/>
@@ -2685,35 +2611,39 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1050357</v>
+        <v>1051391</v>
       </c>
       <c r="B60" t="b">
         <v>0</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>848796</t>
+          <t>849830</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Subvención al cluba de tenis Santa Ana</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr"/>
+          <t>BASES DE AYUDAS A TRAVÉS DE INCENTIVOS A LA CONTRATACIÓN TEMPORAL POR CUENTA AJENA DE LAS PERSONAS PARTICIPANTES EN EL OBRADOIRO DUAL DE EMPLEO “QUEDA EN MOS III”, DIRIGIDO A EMPRESAS,  PARA OCUPACIONES DEL ÁMBITO DE LA FORMACIÓN IMPARTIDA</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>BASES DE AXUDAS A TRAVÉS DE INCENTIVOS Á CONTRATACIÓN TEMPORAL POR CONTA ALLEA DAS PERSOAS PARTICIPANTES DO OBRADOIRO DUAL DE EMPREGO “QUEDA EN MOS III”, DIRIXIDO A EMPRESAS PARA OCUPACIÓNS DO ÁMBITO DA FORMACIÓN IMPARTIDA</t>
+        </is>
+      </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>HELLÍN</t>
+          <t>MOS</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE HELLÍN</t>
+          <t>AYUNTAMIENTO DE MOS</t>
         </is>
       </c>
       <c r="I60" t="inlineStr"/>
@@ -2721,39 +2651,35 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1050356</v>
+        <v>1051390</v>
       </c>
       <c r="B61" t="b">
         <v>0</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>848795</t>
+          <t>849829</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>PREMIOS ESTUDIANTES. CONVOCATORIA AÑO 2025</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>PREMIS ESTUDIANTS. CONVOCATÒRIA ANY 2025</t>
-        </is>
-      </c>
+          <t>CONVOCATORIA Y BASES ESPECÍFICAS REGULADORAS PARA LA CONCESIÓN DE SUBVENCIONES A DEPORTISTAS Y ENTIDADES DEPORTIVAS DE VEJER DE LA FRONTERA</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>RIUDELLOTS DE LA SELVA</t>
+          <t>VEJER DE LA FRONTERA</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE RIUDELLOTS DE LA SELVA</t>
+          <t>AYUNTAMIENTO DE VEJER DE LA FRONTERA</t>
         </is>
       </c>
       <c r="I61" t="inlineStr"/>
@@ -2761,39 +2687,35 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1050355</v>
+        <v>1051389</v>
       </c>
       <c r="B62" t="b">
         <v>0</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>848794</t>
+          <t>849828</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Convenio de colaboración economica con la Asociación española Contra el Cancer año 2025</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>Conveni de col·laboració econòmica amb l'Associació espanyola Contra el Cancer any 2025</t>
-        </is>
-      </c>
+          <t>JUNTA GOBIERNO DE 30/07/2025 QUE APRUEBA LA CONVOCATORIA DEL CERTAMEN “ALCARRIA LITERARIA”, DENTRO DEL PLAN DE SOSTENIBILIDAD TURÍSTICA DEL MISMO NOMBRE, EN LAS MODALIDADES DE ENSAYO, NARRATIVA DE VIAJES Y PERIODISMO.</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>BELLVEI</t>
+          <t>DIPUTACIÓN PROV. DE GUADALAJARA</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE BELLVEI</t>
+          <t>DIPUTACIÓN PROVINCIAL DE GUADALAJARA</t>
         </is>
       </c>
       <c r="I62" t="inlineStr"/>
@@ -2801,75 +2723,75 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1050354</v>
+        <v>1051388</v>
       </c>
       <c r="B63" t="b">
         <v>0</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>848793</t>
+          <t>849827</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Convenio entre el Ayuntamiento de A Coruña y Club Marineda Atlético para Fomento y Promoción del Atletismo.</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>Convenio entre o Concello da Coruña e Club Marineda Atlético para Fomento e Promoción do Atletismo.</t>
-        </is>
-      </c>
+          <t>RESOLUCION DE LA DIRECTORA GERENTE DEL INSTITUTO ARAGONES DE FOMENTO, POR LA QUE SE CONCEDE SUBVENCION NOMINATIVA A LA FUNDACION SANTA MARIA DE ALBARRACIN PARA EL EJERCICIO 2023, PARA GASTOS CORRIENTES DERIVADOS DE SU GESTION</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>CORUÑA, A</t>
+          <t>ARAGÓN</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE CORUÑA, A</t>
+          <t>INSTITUTO ARAGONÉS DE FOMENTO (IAF)</t>
         </is>
       </c>
       <c r="I63" t="inlineStr"/>
-      <c r="J63" t="inlineStr"/>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>INV00003653</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>1050353</v>
+        <v>1051387</v>
       </c>
       <c r="B64" t="b">
         <v>0</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>848792</t>
+          <t>849826</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>CONVENIO DE COLABORACIÓN ENTRE EL AYUNTAMIENTO DE TOTANA Y LA PARROQUIA DE LAS TREA AVEMARÍAS DE TOTANA PARA LA REALIZACIÓN DE ACCIONES DE INTERÉS SOCIAL DESARROLLADAS POR CÁRITAS PARROQUIAL EN EL MUNICIPIO DE TOTANA.- AÑO 2025</t>
+          <t>ADENDA 2025 AL CONVENIO 2024-25 ENTRE LA FMSS DEL AYTO DE GIJON E INTGRAF SC</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>TOTANA</t>
+          <t>GIJÓN</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE TOTANA</t>
+          <t>AYUNTAMIENTO DE GIJÓN</t>
         </is>
       </c>
       <c r="I64" t="inlineStr"/>
@@ -2877,75 +2799,83 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>1050352</v>
+        <v>1051386</v>
       </c>
       <c r="B65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>848791</t>
+          <t>849825</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>PREMIOS EXDUCERE 2025</t>
+          <t>Resolución de 29 de mayo de 2025 del Consejo Rector de la SETT por la que se convocan préstamos para financiar proyectos de transformación digital y difusión de contenidos para empresas del sector de los medios de comunicación.</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>ZARAGOZA</t>
+          <t>ESTADO</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE ZARAGOZA</t>
-        </is>
-      </c>
-      <c r="I65" t="inlineStr"/>
+          <t>MINISTERIO PARA LA TRANSFORMACIÓN DIGITAL Y DE LA FUNCIÓN PÚBLICA</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>ENTIDAD PÚBLICA EMPRESARIAL SOCIEDAD ESPAÑOLA PARA LA TRANSFORMACIÓN TECNOLÓGICA</t>
+        </is>
+      </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>INV00003559</t>
+          <t>INV00005709</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>1050351</v>
+        <v>1051385</v>
       </c>
       <c r="B66" t="b">
         <v>0</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>848790</t>
+          <t>849824</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>CONVENIO DE COLABORACIÓN ENTRE LA DIPUTACIÓN PROVINCIAL DE PALENCIA Y EL AYUNTAMIENTO DE PALENZUELA PARA LA FERIA DE LA CEBOLLA 2025</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr"/>
+          <t>CONVENIO DE COLABORACIÓN ENTRE EL AYUNTAMIENTO DE SENTMENAT Y LA ASOCIACIÓN CULTURAL CASA DE ANDALUCÍA EN SENTMENAT PARA PROMOVER LA CULTURA ANDALUZA EN SENTMENAT.</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>CONVENI DE COL·LABORACIÓ ENTRE L’AJUNTAMENT DE SENTMENAT I L’ASSOCIACIÓ CULTURAL CASA DE ANDALUCÍA EN SENTMENAT PER TAL DE PROMOURE LA CULTURA ANDALUSA A SENTMENAT.</t>
+        </is>
+      </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>DIPUTACIÓN PROV. DE PALENCIA</t>
+          <t>SENTMENAT</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>DIPUTACIÓN PROVINCIAL DE PALENCIA</t>
+          <t>AYUNTAMIENTO DE SENTMENAT</t>
         </is>
       </c>
       <c r="I66" t="inlineStr"/>
@@ -2953,35 +2883,39 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1050350</v>
+        <v>1051384</v>
       </c>
       <c r="B67" t="b">
         <v>0</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>848789</t>
+          <t>849823</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Subvención directa, con carácter excepcional, para la gestión, organización y coordinación de las actividades culturales en la Plaza de Toros de  Talavera de la Reina</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr"/>
+          <t>Convocatoria de subvención a la entidad PASCUAL ATS MUSIC SLU Sons del Món, ejercicio 2025</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Convocatòria de subvenció a l’entitat PASCUAL ARTS MUSIC SLU, exercici 2025</t>
+        </is>
+      </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>TALAVERA DE LA REINA</t>
+          <t>ROSES</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE TALAVERA DE LA REINA</t>
+          <t>AYUNTAMIENTO DE ROSES</t>
         </is>
       </c>
       <c r="I67" t="inlineStr"/>
@@ -2989,65 +2923,61 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>1050349</v>
+        <v>1051383</v>
       </c>
       <c r="B68" t="b">
         <v>0</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>848788</t>
+          <t>849822</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Ayudas de movilidad al estudiantado de la Universitat Jaume I para la asistencia a cursos, seminarios, estancias de investigación u otras actividades que desarrollan en las universidades de la Xarxa Vives o que participan en el programa DRA</t>
+          <t>Decreto de Presidencia nº 3.727 de 4 de julio 2025, de colaboración con Cámara de Comercio de  Valladolid  para el desarrollo del programa `MEDIACION, año 2025`</t>
         </is>
       </c>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>OTROS</t>
+          <t>DIPUTACIÓN PROV. DE VALLADOLID</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>UNIVERSIDAD JAUME I DE CASTELLÓN</t>
+          <t>DIPUTACIÓN PROVINCIAL DE VALLADOLID</t>
         </is>
       </c>
       <c r="I68" t="inlineStr"/>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>INV00005381</t>
-        </is>
-      </c>
+      <c r="J68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1050348</v>
+        <v>1051382</v>
       </c>
       <c r="B69" t="b">
         <v>0</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>848787</t>
+          <t>849821</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Res. 28-07-2025 vicerrectora de Internacionalización de la Universidad de Oviedo, de ayudas de movilidad internacional de corta duración destinada a estudiantes de Doctorado, curso 2025/26, en instituciones con acuerdos Erasmus+KA131.</t>
+          <t>Becas de iniciación a la investigación del Instituto Universitario de Matemáticas y Aplicaciones de Castellon (IMAC)</t>
         </is>
       </c>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -3057,47 +2987,51 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>UNIVERSIDAD DE OVIEDO</t>
+          <t>UNIVERSIDAD JAUME I DE CASTELLÓN</t>
         </is>
       </c>
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr">
         <is>
-          <t>INV00005347</t>
+          <t>INV00005381</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>1050347</v>
+        <v>1051381</v>
       </c>
       <c r="B70" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>848786</t>
+          <t>849820</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>MRR C19 I1 CAPACITACIÓN DIGITAL ASOCIACIONES Y ENTIDADES DEPORTIVAS</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr"/>
+          <t>Convenio entre el Ayuntamiento de A Coruña y el Club Natación Coruña para Fomento y Promoción de la Natación.</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Convenio entre o Concello da Coruña e Club Natación Coruña para Fomento e Promoción da Natación.</t>
+        </is>
+      </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>COMUNIDAD DE MADRID</t>
+          <t>CORUÑA, A</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>CONSEJERÍA DE DIGITALIZACIÓN</t>
+          <t>AYUNTAMIENTO DE CORUÑA, A</t>
         </is>
       </c>
       <c r="I70" t="inlineStr"/>
@@ -3105,39 +3039,35 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>1050346</v>
+        <v>1051378</v>
       </c>
       <c r="B71" t="b">
         <v>0</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>848785</t>
+          <t>849817</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>RESOLUCIÓN de 17 de julio de 2025, por la que se conceden ayudas a la Fundación Valenciana Premios Rei Jaume I de la Comunitat Valenciana (línea de subvención S0664) para el ejercicio 2025.</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>RESOLUCIÓ de 17 de juliol de 2025, per la qual es concedixen ajudes a la Fundació Valenciana Premis Rei Jaume I de la Comunitat Valenciana (línia de subvenció S0664) per a l’exercici 2025.</t>
-        </is>
-      </c>
+          <t>Convocatorias de ayudas para la adquisición de material escolar. Curso 2025-2026</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>COMUNITAT VALENCIANA</t>
+          <t>SALAMANCA</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>SECRETARIA AUTONÓMICA DEL GABINETE DEL PRESIDENT Y COMUNICACIÓN</t>
+          <t>AYUNTAMIENTO DE SALAMANCA</t>
         </is>
       </c>
       <c r="I71" t="inlineStr"/>
@@ -3145,29 +3075,29 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>1050345</v>
+        <v>1051377</v>
       </c>
       <c r="B72" t="b">
         <v>0</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>848784</t>
+          <t>849816</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Convenio entre el ayuntamiento de A coruña y el Club Hércules XTRM para fomento y promoción del Triatlón</t>
+          <t>Convenio entre el Ayuntamiento de A Coruña y el Club Maristas A Coruña para Fomento y Promoción del Baloncesto.</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Convenio entre o Concello de A Coruña y el Club Hércules XTRM para o fomento e promoción do Triatlón.</t>
+          <t>Convenio entre o Concello da Coruña e Club Maristas A Coruña para Fomento e Promoción do Baloncesto.</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -3185,35 +3115,35 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>1050344</v>
+        <v>1051376</v>
       </c>
       <c r="B73" t="b">
         <v>0</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>848783</t>
+          <t>849815</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>AYUDA EMERGENCIA ALQUILER JULIO 2025</t>
+          <t>SUBV. NOMINATIVA A LA REAL PIADOSA CONGREGACIÓN DE SAN CIRIACO Y SANTA PAULA PATRONOS DE MÁLAGA, PARA EL PROYECTO "DESFILE PROCESIONAL 2025"</t>
         </is>
       </c>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>HUELVA</t>
+          <t>MÁLAGA</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE HUELVA</t>
+          <t>AYUNTAMIENTO DE MÁLAGA</t>
         </is>
       </c>
       <c r="I73" t="inlineStr"/>
@@ -3221,75 +3151,75 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>1050342</v>
+        <v>1051375</v>
       </c>
       <c r="B74" t="b">
         <v>0</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>848781</t>
+          <t>849814</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Subvención al Ayuntamiento de Chia para la reparación y acondicionamiento de la pista Chía-Sahún</t>
+          <t>5/2025 CONVENIO ENTRE EL PMD Y CLUB INTERNACIONAL DE LA AMISTAD PRA LA PROMCION DEL DEPORTE BASE Y LA UTILIZACION DE SUS CAMPOS</t>
         </is>
       </c>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>DIPUTACIÓN PROV. DE HUESCA</t>
+          <t>PALENCIA</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>DIPUTACIÓN PROVINCIAL DE HUESCA</t>
+          <t>PATRONATO MUNICIPAL DE DEPORTES</t>
         </is>
       </c>
       <c r="I74" t="inlineStr"/>
-      <c r="J74" t="inlineStr"/>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>INV00004314</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>1050341</v>
+        <v>1051374</v>
       </c>
       <c r="B75" t="b">
         <v>0</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>848780</t>
+          <t>849813</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Subvención concesión directa a l'Escola Gimnàstica Rítmica Pals</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>Subvenció concessió directa a l'Escola Gimnàstica Rítmica Pals</t>
-        </is>
-      </c>
+          <t>INSTALACIÓN DE PROTECCIÓN SOLAT (TOLDO) EN EL COLEGIO ZURBARÁN DE DON BENITO</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>PALS</t>
+          <t>DON BENITO</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>AYUNTAMIENTO DE PALS</t>
+          <t>AYUNTAMIENTO DE DON BENITO</t>
         </is>
       </c>
       <c r="I75" t="inlineStr"/>
@@ -3297,43 +3227,43 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1050340</v>
+        <v>1051373</v>
       </c>
       <c r="B76" t="b">
         <v>0</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>848779</t>
+          <t>849812</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Ayudas de movilidad al profesorado universitario de la Universitat Jaume I para realizar estancias durante el curso académico 2025-2026 en las universidades de la Xarxa Vives o participantes en el programa DRAC.</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr"/>
+          <t>Convenio entre el Ayuntamiento de A Coruña y el Club Polideportivo Esclavas para fomento y promoción del Fútbol y baloncesto.</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Convenio entre o Concello da Coruña e o Club Polideportivo Escravas para fomento e promoción do fútbol e baloncesto.</t>
+        </is>
+      </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>OTROS</t>
+          <t>CORUÑA, A</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>UNIVERSIDAD JAUME I DE CASTELLÓN</t>
+          <t>AYUNTAMIENTO DE CORUÑA, A</t>
         </is>
       </c>
       <c r="I76" t="inlineStr"/>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>INV00005381</t>
-        </is>
-      </c>
+      <c r="J76" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>